<commit_message>
Matrix scanning prelim works
Also adds a GPIO CubeMx project for GPIO inititalization
</commit_message>
<xml_diff>
--- a/USB_Device_Pin_Assignment.xlsx
+++ b/USB_Device_Pin_Assignment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\White_Dove_Keyboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dove_keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4A529C-1DF1-4385-9DA9-A9B2336D1803}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F64219-7553-4238-B000-8DCE946DB294}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{9159E91A-B67A-4120-8F5C-5374B678DA23}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
   <si>
     <t>Port A</t>
   </si>
@@ -710,7 +710,7 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,9 +794,6 @@
       <c r="G5" t="s">
         <v>41</v>
       </c>
-      <c r="I5" t="s">
-        <v>63</v>
-      </c>
       <c r="J5" s="5" t="s">
         <v>77</v>
       </c>
@@ -824,9 +821,6 @@
       <c r="G6" t="s">
         <v>41</v>
       </c>
-      <c r="I6" t="s">
-        <v>64</v>
-      </c>
       <c r="J6" s="5" t="s">
         <v>77</v>
       </c>
@@ -853,9 +847,6 @@
       </c>
       <c r="G7" t="s">
         <v>59</v>
-      </c>
-      <c r="I7" t="s">
-        <v>81</v>
       </c>
       <c r="L7" t="s">
         <v>81</v>
@@ -1567,7 +1558,7 @@
       <c r="G41" t="s">
         <v>43</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="2" t="s">
         <v>63</v>
       </c>
       <c r="L41" s="5" t="s">
@@ -1590,7 +1581,7 @@
       <c r="G42" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="2" t="s">
         <v>64</v>
       </c>
       <c r="L42" s="5" t="s">
@@ -1613,7 +1604,7 @@
       <c r="G43" t="s">
         <v>43</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I43" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L43" s="5" t="s">

</xml_diff>